<commit_message>
cleared out the data file
</commit_message>
<xml_diff>
--- a/Utils/Data/data_model.xlsx
+++ b/Utils/Data/data_model.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Admin/Documents/GitHub/banner_magic/Utils/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{507CB2CF-73D6-2047-880E-E21D8B4FA0A4}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7B01C9D-5669-A84D-8875-A269EDE9149A}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -344,7 +344,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection sqref="A1:B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
reset the the standard v-1.1.0
</commit_message>
<xml_diff>
--- a/Utils/Data/data_model.xlsx
+++ b/Utils/Data/data_model.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Admin/Documents/GitHub/banner_magic/Utils/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E81EA65D-9C98-EF49-A777-D9572CC6D8AC}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5E17725-1431-9940-B265-4A2D3E74E61A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14700" yWindow="-20920" windowWidth="31660" windowHeight="16700" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13900" yWindow="-19780" windowWidth="34380" windowHeight="16580" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,30 +25,87 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <si>
-    <t>Title 1</t>
-  </si>
-  <si>
-    <t>Title 2</t>
-  </si>
-  <si>
-    <t>Price was/from</t>
-  </si>
-  <si>
-    <t>Price is</t>
-  </si>
-  <si>
-    <t>Image path</t>
-  </si>
-  <si>
-    <t>CTA</t>
-  </si>
-  <si>
-    <t>Saving</t>
-  </si>
-  <si>
-    <t>Link</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="27">
+  <si>
+    <t>Cooling</t>
+  </si>
+  <si>
+    <t>Radiators</t>
+  </si>
+  <si>
+    <t>Controls</t>
+  </si>
+  <si>
+    <t>Cylinders</t>
+  </si>
+  <si>
+    <t>Showers</t>
+  </si>
+  <si>
+    <t>Fittings</t>
+  </si>
+  <si>
+    <t>Ventilation</t>
+  </si>
+  <si>
+    <t>Kitchen</t>
+  </si>
+  <si>
+    <t>up to</t>
+  </si>
+  <si>
+    <t>over</t>
+  </si>
+  <si>
+    <t>35%</t>
+  </si>
+  <si>
+    <t>40%</t>
+  </si>
+  <si>
+    <t>25%</t>
+  </si>
+  <si>
+    <t>30%</t>
+  </si>
+  <si>
+    <t>60%</t>
+  </si>
+  <si>
+    <t>50%</t>
+  </si>
+  <si>
+    <t>65%</t>
+  </si>
+  <si>
+    <t>15%</t>
+  </si>
+  <si>
+    <t>Water treatment</t>
+  </si>
+  <si>
+    <t>Water heaters</t>
+  </si>
+  <si>
+    <t>Heating pumps</t>
+  </si>
+  <si>
+    <t>Enclosures &amp; trays</t>
+  </si>
+  <si>
+    <t>Drainage &amp; ufh</t>
+  </si>
+  <si>
+    <t>Power tools</t>
+  </si>
+  <si>
+    <t>Hand tools</t>
+  </si>
+  <si>
+    <t>Trade essentials</t>
+  </si>
+  <si>
+    <t>Bathrooms suites</t>
   </si>
 </sst>
 </file>
@@ -64,29 +121,22 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="12"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -94,30 +144,14 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -398,43 +432,205 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.5" customWidth="1"/>
-    <col min="6" max="6" width="11.6640625" customWidth="1"/>
+    <col min="1" max="1" width="21.5" customWidth="1"/>
+    <col min="2" max="2" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="B12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="B16" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
         <v>7</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>